<commit_message>
add clustering, add prosumer battery storage model, change demand elasticity back to 1 value
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing_v3.xlsx
+++ b/model/model_inputs_testing_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED2E060-A163-4DEE-9948-32062468E668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE04A8B-0C70-4629-A403-7EE65435F5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -296,6 +296,1746 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'elec_demand (1)'!$B$2:$Y$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-057D-422A-9B0F-1C7A4F579CE9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="164066111"/>
+        <c:axId val="164066527"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="164066111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="164066527"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="164066527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="164066111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8928258967629044E-2"/>
+          <c:y val="0.16245370370370371"/>
+          <c:w val="0.8966272965879265"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'elec_demand (1)'!$B$3:$Y$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-79C3-4308-BBD4-381C4DAEB75F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2132628863"/>
+        <c:axId val="2132632607"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2132628863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2132632607"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2132632607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2132628863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -711,6 +2451,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{122FBC7A-822A-4054-B853-F86505FC4C38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E173C4A0-0321-4C1A-ADA7-0957CC54BD8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1031,7 +2848,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1105,7 +2922,7 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y4"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1541,6 +3358,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1548,7 +3366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867F374D-6AFF-43B6-B370-B2ECC1DAC459}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
@@ -1990,7 +3808,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2051,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2114,10 +3932,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>430</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <v>20</v>
@@ -2160,7 +3978,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -2473,7 +4291,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2493,7 +4311,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>150</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -2710,7 +4528,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2804,52 +4622,52 @@
         <v>0</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>0.02</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>0.15</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>0.34</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>0.5</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>0.63</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>0.7</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>0.73</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>0.72</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>0.66</v>
       </c>
-      <c r="M2">
+      <c r="P2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="N2">
+      <c r="Q2">
         <v>0.4</v>
       </c>
-      <c r="O2">
+      <c r="R2">
         <v>0.21</v>
       </c>
-      <c r="P2">
+      <c r="S2">
         <v>0.05</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -2884,49 +4702,49 @@
         <v>0</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>0.12</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>0.33</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>0.51</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>0.65</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>0.73</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>0.76</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>0.74</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>0.68</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="N3">
+      <c r="Q3">
         <v>0.39</v>
       </c>
-      <c r="O3">
+      <c r="R3">
         <v>0.19</v>
       </c>
-      <c r="P3">
+      <c r="S3">
         <v>0.02</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -2964,40 +4782,40 @@
         <v>0</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>0.16</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.35</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.49</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>0.61</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>0.49</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>0.36</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>0.19</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>0.03</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>

</xml_diff>

<commit_message>
add restricition on pv area and restricition on feed in energy and unmet Demand
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing_v3.xlsx
+++ b/model/model_inputs_testing_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53885656-9E46-41E3-B747-7363C4D27D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDDA880-316F-43D7-89E8-5FB43792FDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -3869,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4527,8 +4527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE7DE72-C341-45B3-B73B-C7F84D832AAF}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
generate pros unmet demand and wasted energy table
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing_v3.xlsx
+++ b/model/model_inputs_testing_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDDA880-316F-43D7-89E8-5FB43792FDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CEDBFD-99E7-4C3A-AB5E-DAD7F9F5F1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -3869,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3909,7 +3909,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="1">
         <v>5</v>
@@ -4006,7 +4006,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4527,7 +4527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE7DE72-C341-45B3-B73B-C7F84D832AAF}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>